<commit_message>
update with "window" step
</commit_message>
<xml_diff>
--- a/src/InputExcell/InputData.xlsx
+++ b/src/InputExcell/InputData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python Projects\Scrapper\src\InputExcell\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA53BA99-E3FB-464B-A2F7-4412E681F3A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E7EEFF1-306F-40BE-8D4D-8EA127B11F2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Roma</t>
   </si>
@@ -85,6 +85,15 @@
   </si>
   <si>
     <t>https://www.isotra.cz</t>
+  </si>
+  <si>
+    <t>window</t>
+  </si>
+  <si>
+    <t>https://www.google.com/</t>
+  </si>
+  <si>
+    <t>GOOGLE</t>
   </si>
 </sst>
 </file>
@@ -402,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -414,7 +423,7 @@
     <col min="3" max="3" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -427,8 +436,11 @@
       <c r="D1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -439,7 +451,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -450,7 +462,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -461,7 +473,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -472,7 +484,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -483,7 +495,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -494,7 +506,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -505,7 +517,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -514,6 +526,17 @@
       </c>
       <c r="C9" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>